<commit_message>
more readable output for remaining courses (added id to title conversion)
</commit_message>
<xml_diff>
--- a/cs_degree_planner/forecast/usercourseTEST/recommendcourses.xlsx
+++ b/cs_degree_planner/forecast/usercourseTEST/recommendcourses.xlsx
@@ -557,7 +557,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>2100.0</v>
+        <v>21000.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>2110.0</v>
+        <v>21100.0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>2120.0</v>
+        <v>21200.0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>3130.0</v>
+        <v>31300.0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>3140.0</v>
+        <v>31400.0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>3150.0</v>
+        <v>31500.0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>3330.0</v>
+        <v>33300.0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>3220.0</v>
+        <v>32200.0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>4430.0</v>
+        <v>44300.0</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>4510.0</v>
+        <v>45100.0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>4530.0</v>
+        <v>45300.0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>41001.0</v>
+        <v>410001.0</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>41002.0</v>
+        <v>410002.0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>41003.0</v>
+        <v>410003.0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>10</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>3300.0</v>
+        <v>33000.0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>4220.0</v>
+        <v>42200.0</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>10</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>4410.0</v>
+        <v>44100.0</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>10</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>4360.0</v>
+        <v>43600.0</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>10</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>4320.0</v>
+        <v>43200.0</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>10</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>4310.0</v>
+        <v>43100.0</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>10</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>4290.0</v>
+        <v>429000.0</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>10</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>4450.0</v>
+        <v>44500.0</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>10</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>4150.0</v>
+        <v>41500.0</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>10</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>4710.0</v>
+        <v>47100.0</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>10</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>4720.0</v>
+        <v>47200.0</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>10</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <v>4250.0</v>
+        <v>42500.0</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>10</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <v>4130.0</v>
+        <v>41300.0</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>10</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <v>4200.0</v>
+        <v>42000.0</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>10</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <v>4730.0</v>
+        <v>47300.0</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>10</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>4230.0</v>
+        <v>42300.0</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>10</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>4610.0</v>
+        <v>46100.0</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>10</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>4330.0</v>
+        <v>43300.0</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>10</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>4340.0</v>
+        <v>43400.0</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>10</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>2311.0</v>
+        <v>23101.0</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>58</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>2321.0</v>
+        <v>23201.0</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>58</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>2511.0</v>
+        <v>25101.0</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>58</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1">
-        <v>2521.0</v>
+        <v>25201.0</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
added more to coursestest
generate forecast has inf loop bc excel is not filled out
</commit_message>
<xml_diff>
--- a/cs_degree_planner/forecast/usercourseTEST/recommendcourses.xlsx
+++ b/cs_degree_planner/forecast/usercourseTEST/recommendcourses.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -128,7 +128,7 @@
     <t>Computer Science III</t>
   </si>
   <si>
-    <t>2120, 2321</t>
+    <t>21200, 23210</t>
   </si>
   <si>
     <t>Intermediate Data Structures</t>
@@ -155,16 +155,19 @@
     <t>User Interfaces</t>
   </si>
   <si>
-    <t>3140, 3130</t>
+    <t>31400, 31300</t>
   </si>
   <si>
     <t>Database Processing</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Data Mining</t>
   </si>
   <si>
-    <t>3130, 3140</t>
+    <t>31300, 31400</t>
   </si>
   <si>
     <t>Computational Science</t>
@@ -200,13 +203,13 @@
     <t>Intro to Parallel Computing</t>
   </si>
   <si>
-    <t>3300, 3130</t>
+    <t>33000, 31300</t>
   </si>
   <si>
     <t>Computer Architecture</t>
   </si>
   <si>
-    <t>3300, 3150</t>
+    <t>33000, 31500</t>
   </si>
   <si>
     <t>Modeling and Simulation</t>
@@ -236,7 +239,7 @@
     <t>Software Methology II</t>
   </si>
   <si>
-    <t>3140, 4250</t>
+    <t>31400, 42500</t>
   </si>
   <si>
     <t>Introduction to Compilers</t>
@@ -245,7 +248,7 @@
     <t>Computer and Network Security</t>
   </si>
   <si>
-    <t>4330, 4320</t>
+    <t>43300, 43200</t>
   </si>
   <si>
     <t>Computer and Network Security II</t>
@@ -264,13 +267,34 @@
   </si>
   <si>
     <t>Calculus II</t>
+  </si>
+  <si>
+    <t>Statistical Models/Methods</t>
+  </si>
+  <si>
+    <t>Elementary Linear Algebra I</t>
+  </si>
+  <si>
+    <t>Elementary Linear Algebra II</t>
+  </si>
+  <si>
+    <t>Calculus for the Biological Sciences I</t>
+  </si>
+  <si>
+    <t>Calculus for the Biological Sciences II</t>
+  </si>
+  <si>
+    <t>Calculus with Theory I</t>
+  </si>
+  <si>
+    <t>Calculus with Theory II</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -281,6 +305,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF312B2C"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -297,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -306,6 +334,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,7 +626,7 @@
         <v>211.0</v>
       </c>
       <c r="D3" s="1">
-        <v>2100.0</v>
+        <v>21000.0</v>
       </c>
       <c r="E3" s="1">
         <v>4.0</v>
@@ -624,7 +655,7 @@
         <v>212.0</v>
       </c>
       <c r="D4" s="1">
-        <v>2110.0</v>
+        <v>21100.0</v>
       </c>
       <c r="E4" s="1">
         <v>4.0</v>
@@ -682,7 +713,7 @@
         <v>314.0</v>
       </c>
       <c r="D6" s="1">
-        <v>2120.0</v>
+        <v>21200.0</v>
       </c>
       <c r="E6" s="1">
         <v>4.0</v>
@@ -711,7 +742,7 @@
         <v>315.0</v>
       </c>
       <c r="D7" s="1">
-        <v>3130.0</v>
+        <v>31300.0</v>
       </c>
       <c r="E7" s="1">
         <v>4.0</v>
@@ -740,7 +771,7 @@
         <v>333.0</v>
       </c>
       <c r="D8" s="1">
-        <v>2120.0</v>
+        <v>21200.0</v>
       </c>
       <c r="E8" s="1">
         <v>4.0</v>
@@ -769,7 +800,7 @@
         <v>322.0</v>
       </c>
       <c r="D9" s="1">
-        <v>2120.0</v>
+        <v>21200.0</v>
       </c>
       <c r="E9" s="1">
         <v>4.0</v>
@@ -798,7 +829,7 @@
         <v>443.0</v>
       </c>
       <c r="D10" s="1">
-        <v>3130.0</v>
+        <v>31300.0</v>
       </c>
       <c r="E10" s="1">
         <v>4.0</v>
@@ -856,13 +887,19 @@
         <v>453.0</v>
       </c>
       <c r="D12" s="1">
-        <v>4510.0</v>
+        <v>45100.0</v>
       </c>
       <c r="E12" s="1">
         <v>4.0</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>0</v>
@@ -879,7 +916,7 @@
         <v>410.0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1">
         <v>4.0</v>
@@ -891,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>0</v>
@@ -911,13 +948,13 @@
         <v>4.0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>0</v>
@@ -943,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I15" s="1" t="b">
         <v>0</v>
@@ -960,7 +997,7 @@
         <v>330.0</v>
       </c>
       <c r="D16" s="1">
-        <v>3140.0</v>
+        <v>31400.0</v>
       </c>
       <c r="E16" s="1">
         <v>4.0</v>
@@ -972,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>1</v>
@@ -989,19 +1026,19 @@
         <v>422.0</v>
       </c>
       <c r="D17" s="1">
-        <v>3130.0</v>
+        <v>31300.0</v>
       </c>
       <c r="E17" s="1">
         <v>4.0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G17" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>1</v>
@@ -1018,7 +1055,7 @@
         <v>441.0</v>
       </c>
       <c r="D18" s="1">
-        <v>3300.0</v>
+        <v>33000.0</v>
       </c>
       <c r="E18" s="1">
         <v>4.0</v>
@@ -1030,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>0</v>
@@ -1047,13 +1084,19 @@
         <v>436.0</v>
       </c>
       <c r="D19" s="1">
-        <v>3300.0</v>
+        <v>33000.0</v>
       </c>
       <c r="E19" s="1">
         <v>4.0</v>
       </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H19" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>0</v>
@@ -1070,7 +1113,7 @@
         <v>432.0</v>
       </c>
       <c r="D20" s="1">
-        <v>3300.0</v>
+        <v>33000.0</v>
       </c>
       <c r="E20" s="1">
         <v>4.0</v>
@@ -1082,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I20" s="1" t="b">
         <v>0</v>
@@ -1099,13 +1142,19 @@
         <v>431.0</v>
       </c>
       <c r="D21" s="1">
-        <v>3300.0</v>
+        <v>33000.0</v>
       </c>
       <c r="E21" s="1">
         <v>4.0</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H21" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>0</v>
@@ -1122,13 +1171,19 @@
         <v>429.0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1">
         <v>4.0</v>
       </c>
+      <c r="F22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H22" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>0</v>
@@ -1145,13 +1200,19 @@
         <v>445.0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E23" s="1">
         <v>4.0</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H23" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I23" s="1" t="b">
         <v>0</v>
@@ -1168,7 +1229,7 @@
         <v>415.0</v>
       </c>
       <c r="D24" s="1">
-        <v>3300.0</v>
+        <v>33000.0</v>
       </c>
       <c r="E24" s="1">
         <v>4.0</v>
@@ -1180,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>1</v>
@@ -1197,7 +1258,7 @@
         <v>471.0</v>
       </c>
       <c r="D25" s="1">
-        <v>3150.0</v>
+        <v>31500.0</v>
       </c>
       <c r="E25" s="1">
         <v>4.0</v>
@@ -1209,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>0</v>
@@ -1226,7 +1287,7 @@
         <v>472.0</v>
       </c>
       <c r="D26" s="1">
-        <v>3150.0</v>
+        <v>31500.0</v>
       </c>
       <c r="E26" s="1">
         <v>4.0</v>
@@ -1238,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I26" s="1" t="b">
         <v>0</v>
@@ -1255,7 +1316,7 @@
         <v>425.0</v>
       </c>
       <c r="D27" s="1">
-        <v>3150.0</v>
+        <v>31500.0</v>
       </c>
       <c r="E27" s="1">
         <v>4.0</v>
@@ -1267,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>1</v>
@@ -1284,19 +1345,19 @@
         <v>413.0</v>
       </c>
       <c r="D28" s="1">
-        <v>3150.0</v>
+        <v>31500.0</v>
       </c>
       <c r="E28" s="1">
         <v>4.0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>0</v>
@@ -1313,13 +1374,19 @@
         <v>420.0</v>
       </c>
       <c r="D29" s="1">
-        <v>3150.0</v>
+        <v>31500.0</v>
       </c>
       <c r="E29" s="1">
         <v>4.0</v>
       </c>
+      <c r="F29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H29" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>0</v>
@@ -1336,13 +1403,19 @@
         <v>473.0</v>
       </c>
       <c r="D30" s="1">
-        <v>3150.0</v>
+        <v>31500.0</v>
       </c>
       <c r="E30" s="1">
         <v>4.0</v>
       </c>
+      <c r="F30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H30" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I30" s="1" t="b">
         <v>0</v>
@@ -1359,7 +1432,7 @@
         <v>423.0</v>
       </c>
       <c r="D31" s="1">
-        <v>4220.0</v>
+        <v>42200.0</v>
       </c>
       <c r="E31" s="1">
         <v>4.0</v>
@@ -1371,7 +1444,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>0</v>
@@ -1388,13 +1461,19 @@
         <v>461.0</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E32" s="1">
         <v>4.0</v>
       </c>
+      <c r="F32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H32" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I32" s="1" t="b">
         <v>0</v>
@@ -1411,19 +1490,19 @@
         <v>433.0</v>
       </c>
       <c r="D33" s="1">
-        <v>4150.0</v>
+        <v>41500.0</v>
       </c>
       <c r="E33" s="1">
         <v>4.0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G33" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I33" s="1" t="b">
         <v>0</v>
@@ -1440,13 +1519,19 @@
         <v>434.0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E34" s="1">
         <v>4.0</v>
       </c>
+      <c r="F34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="H34" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>0</v>
@@ -1457,22 +1542,25 @@
         <v>23101.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C35" s="1">
         <v>231.0</v>
       </c>
       <c r="D35" s="1">
-        <v>1121.0</v>
+        <v>11201.0</v>
       </c>
       <c r="E35" s="1">
         <v>4.0</v>
       </c>
+      <c r="F35" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G35" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I35" s="1" t="b">
         <v>1</v>
@@ -1483,22 +1571,25 @@
         <v>23201.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C36" s="1">
         <v>232.0</v>
       </c>
       <c r="D36" s="1">
-        <v>2311.0</v>
+        <v>23101.0</v>
       </c>
       <c r="E36" s="1">
         <v>4.0</v>
       </c>
+      <c r="F36" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
@@ -1509,22 +1600,25 @@
         <v>25101.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C37" s="1">
         <v>251.0</v>
       </c>
       <c r="D37" s="1">
-        <v>1121.0</v>
+        <v>11201.0</v>
       </c>
       <c r="E37" s="1">
         <v>4.0</v>
       </c>
+      <c r="F37" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I37" s="1" t="b">
         <v>0</v>
@@ -1535,24 +1629,218 @@
         <v>25201.0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1">
         <v>252.0</v>
       </c>
       <c r="D38" s="1">
-        <v>2511.0</v>
+        <v>25101.0</v>
       </c>
       <c r="E38" s="1">
         <v>4.0</v>
       </c>
+      <c r="F38" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I38" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1">
+        <v>34301.0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="1">
+        <v>343.0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>25201.0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I39" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1">
+        <v>34101.0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="1">
+        <v>341.0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>25201.0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1">
+        <v>34201.0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="1">
+        <v>342.0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>34101.0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I41" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1">
+        <v>24601.0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="1">
+        <v>246.0</v>
+      </c>
+      <c r="D42" s="1">
+        <v>11201.0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I42" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>24701.0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="1">
+        <v>247.0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>24601.0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I43" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1">
+        <v>26101.0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="1">
+        <v>261.0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1">
+        <v>26201.0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="1">
+        <v>262.0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I45" s="1" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remaining courses list alg done ish, see description
coursestest.py: tons of changes, but basically remaining courses works with extremely minimal testing so far. spreadsheet: many new additions. done ish as far as i know. i think it now has everything we would want to recommend EXCEPT for classes that are not set at 4 credits which have not been added yet
</commit_message>
<xml_diff>
--- a/cs_degree_planner/forecast/usercourseTEST/recommendcourses.xlsx
+++ b/cs_degree_planner/forecast/usercourseTEST/recommendcourses.xlsx
@@ -16,19 +16,19 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C34">
+    <comment authorId="0" ref="C35">
       <text>
         <t xml:space="preserve">may never be offered
 	-ɱᴇᴇᴘᴇґ</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C32">
+    <comment authorId="0" ref="C33">
       <text>
         <t xml:space="preserve">may never be offered
 	-ɱᴇᴇᴘᴇґ</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C30">
+    <comment authorId="0" ref="C31">
       <text>
         <t xml:space="preserve">may never be offered
 	-ɱᴇᴇᴘᴇґ</t>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="151">
   <si>
     <t>id</t>
   </si>
@@ -107,6 +107,9 @@
     <t>keywords</t>
   </si>
   <si>
+    <t>satisfyarea</t>
+  </si>
+  <si>
     <t>CS</t>
   </si>
   <si>
@@ -116,6 +119,9 @@
     <t>Computer Science I</t>
   </si>
   <si>
+    <t>na</t>
+  </si>
+  <si>
     <t>WS</t>
   </si>
   <si>
@@ -128,7 +134,7 @@
     <t>Computer Science III</t>
   </si>
   <si>
-    <t>21200, 23210</t>
+    <t>212000, 232100</t>
   </si>
   <si>
     <t>Intermediate Data Structures</t>
@@ -146,6 +152,9 @@
     <t>Applied Cryptography</t>
   </si>
   <si>
+    <t>cselectiveunder</t>
+  </si>
+  <si>
     <t>Intro to Software Engineering</t>
   </si>
   <si>
@@ -155,7 +164,10 @@
     <t>User Interfaces</t>
   </si>
   <si>
-    <t>31400, 31300</t>
+    <t>cselectiveover</t>
+  </si>
+  <si>
+    <t>314000, 313000</t>
   </si>
   <si>
     <t>Database Processing</t>
@@ -167,7 +179,7 @@
     <t>Data Mining</t>
   </si>
   <si>
-    <t>31300, 31400</t>
+    <t>313000, 314000</t>
   </si>
   <si>
     <t>Computational Science</t>
@@ -203,13 +215,13 @@
     <t>Intro to Parallel Computing</t>
   </si>
   <si>
-    <t>33000, 31300</t>
+    <t>330000, 313000</t>
   </si>
   <si>
     <t>Computer Architecture</t>
   </si>
   <si>
-    <t>33000, 31500</t>
+    <t>330000, 315000</t>
   </si>
   <si>
     <t>Modeling and Simulation</t>
@@ -230,6 +242,9 @@
     <t>Advanced Data Structures</t>
   </si>
   <si>
+    <t>csmath, cselectiveover</t>
+  </si>
+  <si>
     <t>Automata Theory</t>
   </si>
   <si>
@@ -239,7 +254,7 @@
     <t>Software Methology II</t>
   </si>
   <si>
-    <t>31400, 42500</t>
+    <t>314000, 425000</t>
   </si>
   <si>
     <t>Introduction to Compilers</t>
@@ -248,7 +263,7 @@
     <t>Computer and Network Security</t>
   </si>
   <si>
-    <t>43300, 43200</t>
+    <t>433000, 432000</t>
   </si>
   <si>
     <t>Computer and Network Security II</t>
@@ -257,6 +272,9 @@
     <t>MATH</t>
   </si>
   <si>
+    <t>Elementary Functions</t>
+  </si>
+  <si>
     <t>Elements of Discrete Mathematics I</t>
   </si>
   <si>
@@ -288,13 +306,235 @@
   </si>
   <si>
     <t>Calculus with Theory II</t>
+  </si>
+  <si>
+    <t>PHYS</t>
+  </si>
+  <si>
+    <t>General Physics I</t>
+  </si>
+  <si>
+    <t>General Physics II</t>
+  </si>
+  <si>
+    <t>General Physics III</t>
+  </si>
+  <si>
+    <t>Foundations of Physics I</t>
+  </si>
+  <si>
+    <t>Foundations of Physics II</t>
+  </si>
+  <si>
+    <t>Foundations of Physics III</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>General Chemistry I</t>
+  </si>
+  <si>
+    <t>General Chemistry II</t>
+  </si>
+  <si>
+    <t>General Chemistry III</t>
+  </si>
+  <si>
+    <t>GEOG</t>
+  </si>
+  <si>
+    <t>The Natural Environment</t>
+  </si>
+  <si>
+    <t>Climatology</t>
+  </si>
+  <si>
+    <t>Geomorphology</t>
+  </si>
+  <si>
+    <t>Biogeography</t>
+  </si>
+  <si>
+    <t>GEOL</t>
+  </si>
+  <si>
+    <t>Earth's Interior Heat and Dynamics</t>
+  </si>
+  <si>
+    <t>Earth Surface and Environmental Geology</t>
+  </si>
+  <si>
+    <t>Evolution of the Earth</t>
+  </si>
+  <si>
+    <t>PSY</t>
+  </si>
+  <si>
+    <t>Mind and Brain</t>
+  </si>
+  <si>
+    <t>Music and the Brain</t>
+  </si>
+  <si>
+    <t>Scientific Thinking</t>
+  </si>
+  <si>
+    <t>Biopsychology</t>
+  </si>
+  <si>
+    <t>Cognition</t>
+  </si>
+  <si>
+    <t>Introduction to Chemical Principles</t>
+  </si>
+  <si>
+    <t>The Chemistry of Sustainability</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>General Biology I</t>
+  </si>
+  <si>
+    <t>General Biology II</t>
+  </si>
+  <si>
+    <t>General Biology III</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>Composition II</t>
+  </si>
+  <si>
+    <t>Scientific and Technical Writing</t>
+  </si>
+  <si>
+    <t>Business Comunications</t>
+  </si>
+  <si>
+    <t>Calculus III</t>
+  </si>
+  <si>
+    <t>csmath</t>
+  </si>
+  <si>
+    <t>Several-Variable Calculus I</t>
+  </si>
+  <si>
+    <t>Introduction to Differential Equations</t>
+  </si>
+  <si>
+    <t>Several-Variable Calculus II</t>
+  </si>
+  <si>
+    <t>Introduction to Proof</t>
+  </si>
+  <si>
+    <t>Fundamentals of Analysis I</t>
+  </si>
+  <si>
+    <t>Fundamentals of Analysis II</t>
+  </si>
+  <si>
+    <t>Theory of Differential Equations</t>
+  </si>
+  <si>
+    <t>Probability and Statistics for Data Science</t>
+  </si>
+  <si>
+    <t>Fundamentals of Number Theory I</t>
+  </si>
+  <si>
+    <t>Fundamentals of Number Theory II</t>
+  </si>
+  <si>
+    <t>Elementary Numerical Analysis I</t>
+  </si>
+  <si>
+    <t>Elementary Numerical Analysis II</t>
+  </si>
+  <si>
+    <t>Fundamentals of Abstract Algebra I</t>
+  </si>
+  <si>
+    <t>Fundamentals of Abstract Algebra II</t>
+  </si>
+  <si>
+    <t>Geometries from an Advanced Viewpoint I</t>
+  </si>
+  <si>
+    <t>Geometries from an Advanced Viewpoint II</t>
+  </si>
+  <si>
+    <t>History and Applications of Calculus</t>
+  </si>
+  <si>
+    <t>Functions of a Complex Variable I</t>
+  </si>
+  <si>
+    <t>Functions of a Complex Variable II</t>
+  </si>
+  <si>
+    <t>Introduction to Analysis I</t>
+  </si>
+  <si>
+    <t>Introduction to Analysis II</t>
+  </si>
+  <si>
+    <t>Introduction to Analysis III</t>
+  </si>
+  <si>
+    <t>Partial Differential Equations: Fourier Analysis I</t>
+  </si>
+  <si>
+    <t>Partial Differential Equations: Fourier Analysis II</t>
+  </si>
+  <si>
+    <t>Introduction to Topology I</t>
+  </si>
+  <si>
+    <t>Introduction to Topology II</t>
+  </si>
+  <si>
+    <t>Introduction to Differential Geometry</t>
+  </si>
+  <si>
+    <t>Introduction to Topology III</t>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
+  </si>
+  <si>
+    <t>Introduction to Abstract Algebra I</t>
+  </si>
+  <si>
+    <t>Introduction to Abstract Algebra II</t>
+  </si>
+  <si>
+    <t>Introduction to Abstract Algebra III</t>
+  </si>
+  <si>
+    <t>Introduction to Mathematical Methods of Statistics I</t>
+  </si>
+  <si>
+    <t>Introduction to Mathematical Methods of Statistics II</t>
+  </si>
+  <si>
+    <t>Mathematical Methods of Regression Analysis and Analysis of Variance</t>
+  </si>
+  <si>
+    <t>Stochastic Processes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -307,16 +547,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF312B2C"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -325,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -335,7 +585,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -553,6 +806,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="8" max="8" width="17.88"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -585,13 +841,16 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>21000.0</v>
+        <v>210000.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>210.0</v>
@@ -603,343 +862,379 @@
         <v>4.0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>21100.0</v>
+        <v>211000.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>211.0</v>
       </c>
       <c r="D3" s="1">
-        <v>21000.0</v>
+        <v>210000.0</v>
       </c>
       <c r="E3" s="1">
         <v>4.0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>21200.0</v>
+        <v>212000.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>212.0</v>
       </c>
       <c r="D4" s="1">
-        <v>21100.0</v>
+        <v>211000.0</v>
       </c>
       <c r="E4" s="1">
         <v>4.0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>31300.0</v>
+        <v>313000.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>313.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>4.0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>31400.0</v>
+        <v>314000.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
         <v>314.0</v>
       </c>
       <c r="D6" s="1">
-        <v>21200.0</v>
+        <v>212000.0</v>
       </c>
       <c r="E6" s="1">
         <v>4.0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1">
         <v>315.0</v>
       </c>
       <c r="D7" s="1">
-        <v>31300.0</v>
+        <v>313000.0</v>
       </c>
       <c r="E7" s="1">
         <v>4.0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>33300.0</v>
+        <v>333000.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>333.0</v>
       </c>
       <c r="D8" s="1">
-        <v>21200.0</v>
+        <v>212000.0</v>
       </c>
       <c r="E8" s="1">
         <v>4.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>32200.0</v>
+        <v>322000.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
         <v>322.0</v>
       </c>
       <c r="D9" s="1">
-        <v>21200.0</v>
+        <v>212000.0</v>
       </c>
       <c r="E9" s="1">
         <v>4.0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I9" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>44300.0</v>
+        <v>443000.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <v>443.0</v>
       </c>
       <c r="D10" s="1">
-        <v>31300.0</v>
+        <v>313000.0</v>
       </c>
       <c r="E10" s="1">
         <v>4.0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>45100.0</v>
+        <v>451000.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
         <v>451.0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1">
         <v>4.0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I11" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>45300.0</v>
+        <v>453000.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
         <v>453.0</v>
       </c>
       <c r="D12" s="1">
-        <v>45100.0</v>
+        <v>451000.0</v>
       </c>
       <c r="E12" s="1">
         <v>4.0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="I12" s="1" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>410001.0</v>
+        <v>4100001.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>410.0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1">
         <v>4.0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>410002.0</v>
+        <v>4100002.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>410.0</v>
@@ -948,24 +1243,27 @@
         <v>4.0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>410003.0</v>
+        <v>4100003.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1">
         <v>410.0</v>
@@ -974,190 +1272,211 @@
         <v>4.0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I15" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1">
         <v>330.0</v>
       </c>
       <c r="D16" s="1">
-        <v>31400.0</v>
+        <v>314000.0</v>
       </c>
       <c r="E16" s="1">
         <v>4.0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>42200.0</v>
+        <v>422000.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1">
         <v>422.0</v>
       </c>
       <c r="D17" s="1">
-        <v>31300.0</v>
+        <v>313000.0</v>
       </c>
       <c r="E17" s="1">
         <v>4.0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>44100.0</v>
+        <v>441000.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1">
         <v>441.0</v>
       </c>
       <c r="D18" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E18" s="1">
         <v>4.0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>43600.0</v>
+        <v>436000.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1">
         <v>436.0</v>
       </c>
       <c r="D19" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E19" s="1">
         <v>4.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>43200.0</v>
+        <v>432000.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1">
         <v>432.0</v>
       </c>
       <c r="D20" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E20" s="1">
         <v>4.0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G20" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I20" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>43100.0</v>
+        <v>431000.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1">
         <v>431.0</v>
       </c>
       <c r="D21" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E21" s="1">
         <v>4.0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22">
@@ -1165,332 +1484,361 @@
         <v>429000.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1">
         <v>429.0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E22" s="1">
         <v>4.0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>44500.0</v>
+        <v>445000.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1">
         <v>445.0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1">
         <v>4.0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I23" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>41500.0</v>
+        <v>415000.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1">
         <v>415.0</v>
       </c>
       <c r="D24" s="1">
-        <v>33000.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E24" s="1">
         <v>4.0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G24" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>47100.0</v>
+        <v>471000.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1">
         <v>471.0</v>
       </c>
       <c r="D25" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E25" s="1">
         <v>4.0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G25" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>47200.0</v>
+        <v>472000.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1">
         <v>472.0</v>
       </c>
       <c r="D26" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E26" s="1">
         <v>4.0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G26" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="I26" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <v>42500.0</v>
+        <v>425000.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27" s="1">
         <v>425.0</v>
       </c>
       <c r="D27" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E27" s="1">
         <v>4.0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G27" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <v>41300.0</v>
+        <v>413000.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="1">
         <v>413.0</v>
       </c>
       <c r="D28" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E28" s="1">
         <v>4.0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <v>42000.0</v>
+        <v>420000.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="1">
         <v>420.0</v>
       </c>
       <c r="D29" s="1">
-        <v>31500.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E29" s="1">
         <v>4.0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <v>47300.0</v>
+        <v>427000.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" s="1">
-        <v>473.0</v>
-      </c>
-      <c r="D30" s="1">
-        <v>31500.0</v>
-      </c>
+        <v>427.0</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="1">
         <v>4.0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G30" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="H30" s="1"/>
       <c r="I30" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>42300.0</v>
+        <v>473000.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C31" s="1">
-        <v>423.0</v>
+        <v>473.0</v>
       </c>
       <c r="D31" s="1">
-        <v>42200.0</v>
+        <v>315000.0</v>
       </c>
       <c r="E31" s="1">
         <v>4.0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G31" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>46100.0</v>
+        <v>423000.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" s="1">
-        <v>461.0</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>54</v>
+        <v>423.0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>422000.0</v>
       </c>
       <c r="E32" s="1">
         <v>4.0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I32" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>43300.0</v>
+        <v>461000.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C33" s="1">
-        <v>433.0</v>
-      </c>
-      <c r="D33" s="1">
-        <v>41500.0</v>
+        <v>461.0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E33" s="1">
         <v>4.0</v>
@@ -1499,349 +1847,2057 @@
         <v>32</v>
       </c>
       <c r="G33" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I33" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>43400.0</v>
+        <v>433000.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1">
-        <v>434.0</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>57</v>
+        <v>433.0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>415000.0</v>
       </c>
       <c r="E34" s="1">
         <v>4.0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>23101.0</v>
+        <v>434000.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="C35" s="1">
-        <v>231.0</v>
-      </c>
-      <c r="D35" s="1">
-        <v>11201.0</v>
+        <v>434.0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="E35" s="1">
         <v>4.0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G35" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I35" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>23201.0</v>
+        <v>112001.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1">
-        <v>232.0</v>
-      </c>
-      <c r="D36" s="1">
-        <v>23101.0</v>
-      </c>
+        <v>112.0</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="1">
         <v>4.0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>25101.0</v>
+        <v>231001.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1">
-        <v>251.0</v>
+        <v>231.0</v>
       </c>
       <c r="D37" s="1">
-        <v>11201.0</v>
+        <v>112001.0</v>
       </c>
       <c r="E37" s="1">
         <v>4.0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I37" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1">
-        <v>25201.0</v>
+        <v>232001.0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1">
-        <v>252.0</v>
+        <v>232.0</v>
       </c>
       <c r="D38" s="1">
-        <v>25101.0</v>
+        <v>231001.0</v>
       </c>
       <c r="E38" s="1">
         <v>4.0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="I38" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1">
-        <v>34301.0</v>
+        <v>251001.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1">
-        <v>343.0</v>
+        <v>251.0</v>
       </c>
       <c r="D39" s="1">
-        <v>25201.0</v>
+        <v>112001.0</v>
       </c>
       <c r="E39" s="1">
         <v>4.0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="G39" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>64</v>
+      <c r="H39" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="I39" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1">
-        <v>34101.0</v>
+        <v>252001.0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1">
-        <v>341.0</v>
+        <v>252.0</v>
       </c>
       <c r="D40" s="1">
-        <v>25201.0</v>
+        <v>251001.0</v>
       </c>
       <c r="E40" s="1">
         <v>4.0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="G40" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>65</v>
+      <c r="H40" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="I40" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1">
-        <v>34201.0</v>
+        <v>343001.0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C41" s="1">
-        <v>342.0</v>
+        <v>343.0</v>
       </c>
       <c r="D41" s="1">
-        <v>34101.0</v>
+        <v>252001.0</v>
       </c>
       <c r="E41" s="1">
         <v>4.0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G41" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>66</v>
+      <c r="H41" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="I41" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1">
-        <v>24601.0</v>
+        <v>341001.0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C42" s="1">
-        <v>246.0</v>
+        <v>341.0</v>
       </c>
       <c r="D42" s="1">
-        <v>11201.0</v>
+        <v>252001.0</v>
       </c>
       <c r="E42" s="1">
         <v>4.0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G42" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>67</v>
+      <c r="H42" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1">
-        <v>24701.0</v>
+        <v>342001.0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1">
-        <v>247.0</v>
+        <v>342.0</v>
       </c>
       <c r="D43" s="1">
-        <v>24601.0</v>
+        <v>341001.0</v>
       </c>
       <c r="E43" s="1">
         <v>4.0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G43" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>68</v>
+      <c r="H43" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1">
-        <v>26101.0</v>
+        <v>246001.0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C44" s="1">
-        <v>261.0</v>
+        <v>246.0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>112001.0</v>
       </c>
       <c r="E44" s="1">
         <v>4.0</v>
       </c>
+      <c r="F44" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="G44" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1">
-        <v>26201.0</v>
+        <v>247001.0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C45" s="1">
+        <v>247.0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>246001.0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1">
+        <v>261001.0</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="1">
+        <v>261.0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1">
+        <v>262001.0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="1">
         <v>262.0</v>
       </c>
-      <c r="E45" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="G45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I45" s="1" t="b">
-        <v>0</v>
+      <c r="E47" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1">
+        <v>201002.0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I48" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1">
+        <v>202002.0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="1">
+        <v>202.0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I49" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1">
+        <v>203002.0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="1">
+        <v>203.0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1">
+        <v>251002.0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="1">
+        <v>251.0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I51" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1">
+        <v>252002.0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="1">
+        <v>252.0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I52" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1">
+        <v>253002.0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I53" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1">
+        <v>221003.0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="1">
+        <v>221.0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I54" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1">
+        <v>222003.0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C55" s="1">
+        <v>222.0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1">
+        <v>223003.0</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="1">
+        <v>223.0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I56" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1">
+        <v>141004.0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" s="1">
+        <v>141.0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I57" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1">
+        <v>321004.0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="1">
+        <v>321.0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1">
+        <v>322004.0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" s="1">
+        <v>322.0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I59" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1">
+        <v>323004.0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="1">
+        <v>323.0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I60" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1">
+        <v>201005.0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I61" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1">
+        <v>202005.0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" s="1">
+        <v>202.0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1">
+        <v>203005.0</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="1">
+        <v>203.0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I63" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1">
+        <v>201006.0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I64" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1">
+        <v>348006.0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" s="1">
+        <v>348.0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I65" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1">
+        <v>301006.0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" s="1">
+        <v>301.0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I66" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1">
+        <v>304006.0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="1">
+        <v>304.0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I67" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1">
+        <v>305006.0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="1">
+        <v>305.0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I68" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1">
+        <v>111003.0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C69" s="1">
+        <v>111.0</v>
+      </c>
+      <c r="E69" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I69" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1">
+        <v>113003.0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" s="1">
+        <v>113.0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I70" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1">
+        <v>211007.0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" s="1">
+        <v>211.0</v>
+      </c>
+      <c r="E71" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I71" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1">
+        <v>212007.0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C72" s="1">
+        <v>212.0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I72" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1">
+        <v>213007.0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1">
+        <v>121008.0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="1">
+        <v>121.0</v>
+      </c>
+      <c r="D74" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G74" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I74" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1">
+        <v>122008.0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C75" s="1">
+        <v>122.0</v>
+      </c>
+      <c r="D75" s="1">
+        <v>121008.0</v>
+      </c>
+      <c r="E75" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1">
+        <v>320008.0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C76" s="1">
+        <v>320.0</v>
+      </c>
+      <c r="D76" s="1">
+        <v>122008.0</v>
+      </c>
+      <c r="E76" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G76" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I76" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1">
+        <v>321008.0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C77" s="1">
+        <v>321.0</v>
+      </c>
+      <c r="D77" s="1">
+        <v>122008.0</v>
+      </c>
+      <c r="E77" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I77" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1">
+        <v>253001.0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="D78" s="1">
+        <v>252001.0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="G78" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I78" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1">
+        <v>281001.0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" s="1">
+        <v>281.0</v>
+      </c>
+      <c r="D79" s="1">
+        <v>253001.0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I79" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1">
+        <v>256001.0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C80" s="1">
+        <v>256.0</v>
+      </c>
+      <c r="D80" s="1">
+        <v>253001.0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I80" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1">
+        <v>282001.0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" s="1">
+        <v>282.0</v>
+      </c>
+      <c r="D81" s="1">
+        <v>281001.0</v>
+      </c>
+      <c r="E81" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I81" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1">
+        <v>307001.0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" s="1">
+        <v>307.0</v>
+      </c>
+      <c r="D82" s="1">
+        <v>252001.0</v>
+      </c>
+      <c r="E82" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1">
+        <v>316001.0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C83" s="1">
+        <v>316.0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1">
+        <v>317001.0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C84" s="1">
+        <v>317.0</v>
+      </c>
+      <c r="D84" s="1">
+        <v>316001.0</v>
+      </c>
+      <c r="E84" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1">
+        <v>320001.0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="1">
+        <v>320.0</v>
+      </c>
+      <c r="E85" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I85" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1">
+        <v>345001.0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86" s="1">
+        <v>345.0</v>
+      </c>
+      <c r="E86" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I86" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1">
+        <v>347001.0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C87" s="1">
+        <v>347.0</v>
+      </c>
+      <c r="E87" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I87" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1">
+        <v>348001.0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C88" s="1">
+        <v>348.0</v>
+      </c>
+      <c r="D88" s="1">
+        <v>347001.0</v>
+      </c>
+      <c r="E88" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I88" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1">
+        <v>351001.0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C89" s="1">
+        <v>351.0</v>
+      </c>
+      <c r="E89" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I89" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1">
+        <v>352001.0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C90" s="1">
+        <v>352.0</v>
+      </c>
+      <c r="D90" s="1">
+        <v>351001.0</v>
+      </c>
+      <c r="E90" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1">
+        <v>391001.0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C91" s="1">
+        <v>391.0</v>
+      </c>
+      <c r="E91" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I91" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1">
+        <v>392001.0</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C92" s="1">
+        <v>392.0</v>
+      </c>
+      <c r="D92" s="1">
+        <v>391001.0</v>
+      </c>
+      <c r="E92" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I92" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1">
+        <v>394001.0</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C93" s="1">
+        <v>394.0</v>
+      </c>
+      <c r="E93" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1">
+        <v>395001.0</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C94" s="1">
+        <v>395.0</v>
+      </c>
+      <c r="D94" s="1">
+        <v>394001.0</v>
+      </c>
+      <c r="E94" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I94" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1">
+        <v>397001.0</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C95" s="1">
+        <v>397.0</v>
+      </c>
+      <c r="E95" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1">
+        <v>411001.0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" s="1">
+        <v>411.0</v>
+      </c>
+      <c r="E96" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I96" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1">
+        <v>412001.0</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C97" s="1">
+        <v>412.0</v>
+      </c>
+      <c r="E97" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I97" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1">
+        <v>413001.0</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C98" s="1">
+        <v>413.0</v>
+      </c>
+      <c r="E98" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I98" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1">
+        <v>414001.0</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C99" s="1">
+        <v>414.0</v>
+      </c>
+      <c r="E99" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I99" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1">
+        <v>415001.0</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C100" s="1">
+        <v>415.0</v>
+      </c>
+      <c r="E100" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I100" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1">
+        <v>421001.0</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C101" s="1">
+        <v>421.0</v>
+      </c>
+      <c r="E101" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I101" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1">
+        <v>422001.0</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C102" s="1">
+        <v>422.0</v>
+      </c>
+      <c r="E102" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I102" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1">
+        <v>431001.0</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C103" s="1">
+        <v>431.0</v>
+      </c>
+      <c r="E103" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I103" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1">
+        <v>432001.0</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C104" s="1">
+        <v>432.0</v>
+      </c>
+      <c r="E104" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I104" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1">
+        <v>433001.0</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C105" s="1">
+        <v>433.0</v>
+      </c>
+      <c r="E105" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1">
+        <v>434001.0</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C106" s="1">
+        <v>434.0</v>
+      </c>
+      <c r="E106" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I106" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1">
+        <v>441001.0</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C107" s="1">
+        <v>441.0</v>
+      </c>
+      <c r="E107" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I107" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1">
+        <v>444001.0</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C108" s="1">
+        <v>444.0</v>
+      </c>
+      <c r="E108" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I108" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1">
+        <v>445001.0</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C109" s="1">
+        <v>445.0</v>
+      </c>
+      <c r="E109" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I109" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1">
+        <v>446001.0</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C110" s="1">
+        <v>446.0</v>
+      </c>
+      <c r="E110" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I110" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1">
+        <v>461001.0</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C111" s="1">
+        <v>461.0</v>
+      </c>
+      <c r="E111" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I111" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1">
+        <v>462001.0</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C112" s="1">
+        <v>462.0</v>
+      </c>
+      <c r="E112" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I112" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1">
+        <v>463001.0</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C113" s="1">
+        <v>463.0</v>
+      </c>
+      <c r="E113" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I113" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1">
+        <v>467001.0</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C114" s="1">
+        <v>467.0</v>
+      </c>
+      <c r="E114" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I114" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor fixes to coursestest.py and update sheet
</commit_message>
<xml_diff>
--- a/cs_degree_planner/forecast/usercourseTEST/recommendcourses.xlsx
+++ b/cs_degree_planner/forecast/usercourseTEST/recommendcourses.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="188">
   <si>
     <t>id</t>
   </si>
@@ -110,6 +110,9 @@
     <t>satisfyarea</t>
   </si>
   <si>
+    <t>notes</t>
+  </si>
+  <si>
     <t>CS</t>
   </si>
   <si>
@@ -119,6 +122,9 @@
     <t>Computer Science I</t>
   </si>
   <si>
+    <t>~</t>
+  </si>
+  <si>
     <t>na</t>
   </si>
   <si>
@@ -152,18 +158,27 @@
     <t>Applied Cryptography</t>
   </si>
   <si>
+    <t>Cryptography, Cybersecurity</t>
+  </si>
+  <si>
     <t>cselectiveunder</t>
   </si>
   <si>
     <t>Intro to Software Engineering</t>
   </si>
   <si>
+    <t>Software</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
     <t>User Interfaces</t>
   </si>
   <si>
+    <t>UI</t>
+  </si>
+  <si>
     <t>cselectiveover</t>
   </si>
   <si>
@@ -173,27 +188,42 @@
     <t>Database Processing</t>
   </si>
   <si>
+    <t>Databases</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
     <t>Data Mining</t>
   </si>
   <si>
+    <t>AI, Databases</t>
+  </si>
+  <si>
     <t>313000, 314000</t>
   </si>
   <si>
     <t>Computational Science</t>
   </si>
   <si>
+    <t>Software, Databases</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
     <t>Game Programming</t>
   </si>
   <si>
+    <t>Games, Graphics, Teamwork</t>
+  </si>
+  <si>
     <t>Multi-agent Systems</t>
   </si>
   <si>
+    <t>AI</t>
+  </si>
+  <si>
     <t>C/C++ and Unix</t>
   </si>
   <si>
@@ -206,21 +236,36 @@
     <t>Intro Computer Graphics</t>
   </si>
   <si>
+    <t>Graphics</t>
+  </si>
+  <si>
     <t>Secure Software Development</t>
   </si>
   <si>
+    <t>Software, Cybersecurity</t>
+  </si>
+  <si>
     <t>Intro to Networks</t>
   </si>
   <si>
+    <t>Networks, Databases</t>
+  </si>
+  <si>
     <t>Intro to Parallel Computing</t>
   </si>
   <si>
+    <t>HPC</t>
+  </si>
+  <si>
     <t>330000, 313000</t>
   </si>
   <si>
     <t>Computer Architecture</t>
   </si>
   <si>
+    <t>todo</t>
+  </si>
+  <si>
     <t>330000, 315000</t>
   </si>
   <si>
@@ -248,12 +293,18 @@
     <t>Automata Theory</t>
   </si>
   <si>
+    <t>does not exist?</t>
+  </si>
+  <si>
     <t>Probabilistic Methods for Artificial Intelligence</t>
   </si>
   <si>
     <t>Software Methology II</t>
   </si>
   <si>
+    <t>Software, Teamwork</t>
+  </si>
+  <si>
     <t>314000, 425000</t>
   </si>
   <si>
@@ -263,6 +314,9 @@
     <t>Computer and Network Security</t>
   </si>
   <si>
+    <t>Networks, Cybersecurity</t>
+  </si>
+  <si>
     <t>433000, 432000</t>
   </si>
   <si>
@@ -284,12 +338,18 @@
     <t>Calculus I</t>
   </si>
   <si>
+    <t>default if don't like biology</t>
+  </si>
+  <si>
     <t>Calculus II</t>
   </si>
   <si>
     <t>Statistical Models/Methods</t>
   </si>
   <si>
+    <t>Statistics</t>
+  </si>
+  <si>
     <t>Elementary Linear Algebra I</t>
   </si>
   <si>
@@ -299,12 +359,18 @@
     <t>Calculus for the Biological Sciences I</t>
   </si>
   <si>
+    <t>Biology</t>
+  </si>
+  <si>
     <t>Calculus for the Biological Sciences II</t>
   </si>
   <si>
     <t>Calculus with Theory I</t>
   </si>
   <si>
+    <t>do not recommend</t>
+  </si>
+  <si>
     <t>Calculus with Theory II</t>
   </si>
   <si>
@@ -314,6 +380,9 @@
     <t>General Physics I</t>
   </si>
   <si>
+    <t>Physics</t>
+  </si>
+  <si>
     <t>General Physics II</t>
   </si>
   <si>
@@ -323,6 +392,9 @@
     <t>Foundations of Physics I</t>
   </si>
   <si>
+    <t>Physics, Advanced Physics</t>
+  </si>
+  <si>
     <t>Foundations of Physics II</t>
   </si>
   <si>
@@ -335,6 +407,9 @@
     <t>General Chemistry I</t>
   </si>
   <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
     <t>General Chemistry II</t>
   </si>
   <si>
@@ -347,21 +422,36 @@
     <t>The Natural Environment</t>
   </si>
   <si>
+    <t>Geography, Climatology, Biology, Geology</t>
+  </si>
+  <si>
     <t>Climatology</t>
   </si>
   <si>
+    <t>Geography, Climatology</t>
+  </si>
+  <si>
     <t>Geomorphology</t>
   </si>
   <si>
+    <t>Geography, Geology</t>
+  </si>
+  <si>
     <t>Biogeography</t>
   </si>
   <si>
+    <t>Geography, Biology</t>
+  </si>
+  <si>
     <t>GEOL</t>
   </si>
   <si>
     <t>Earth's Interior Heat and Dynamics</t>
   </si>
   <si>
+    <t>Geology</t>
+  </si>
+  <si>
     <t>Earth Surface and Environmental Geology</t>
   </si>
   <si>
@@ -374,15 +464,24 @@
     <t>Mind and Brain</t>
   </si>
   <si>
+    <t>Psychology</t>
+  </si>
+  <si>
     <t>Music and the Brain</t>
   </si>
   <si>
+    <t>Music, Psychology</t>
+  </si>
+  <si>
     <t>Scientific Thinking</t>
   </si>
   <si>
     <t>Biopsychology</t>
   </si>
   <si>
+    <t>Psychology, Biology</t>
+  </si>
+  <si>
     <t>Cognition</t>
   </si>
   <si>
@@ -392,6 +491,9 @@
     <t>The Chemistry of Sustainability</t>
   </si>
   <si>
+    <t>cant find</t>
+  </si>
+  <si>
     <t>BI</t>
   </si>
   <si>
@@ -416,9 +518,15 @@
     <t>Business Comunications</t>
   </si>
   <si>
+    <t>Business</t>
+  </si>
+  <si>
     <t>Calculus III</t>
   </si>
   <si>
+    <t>Calculus</t>
+  </si>
+  <si>
     <t>csmath</t>
   </si>
   <si>
@@ -432,6 +540,9 @@
   </si>
   <si>
     <t>Introduction to Proof</t>
+  </si>
+  <si>
+    <t>Proofs</t>
   </si>
   <si>
     <t>Fundamentals of Analysis I</t>
@@ -582,11 +693,11 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -844,13 +955,16 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>210000.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>210.0</v>
@@ -862,19 +976,22 @@
         <v>4.0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -882,7 +999,7 @@
         <v>211000.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>211.0</v>
@@ -894,19 +1011,22 @@
         <v>4.0</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -914,7 +1034,7 @@
         <v>212000.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>212.0</v>
@@ -926,19 +1046,22 @@
         <v>4.0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -946,31 +1069,34 @@
         <v>313000.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>313.0</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E5" s="1">
         <v>4.0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
@@ -978,7 +1104,7 @@
         <v>314000.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>314.0</v>
@@ -990,19 +1116,22 @@
         <v>4.0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -1010,7 +1139,7 @@
         <v>315000.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
         <v>315.0</v>
@@ -1022,19 +1151,22 @@
         <v>4.0</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -1042,7 +1174,7 @@
         <v>333000.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
         <v>333.0</v>
@@ -1054,19 +1186,22 @@
         <v>4.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J8" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K8" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -1074,7 +1209,7 @@
         <v>322000.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>322.0</v>
@@ -1086,19 +1221,22 @@
         <v>4.0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>25</v>
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1106,7 +1244,7 @@
         <v>443000.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1">
         <v>443.0</v>
@@ -1118,19 +1256,22 @@
         <v>4.0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J10" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="K10" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -1138,31 +1279,34 @@
         <v>451000.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>451.0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1">
         <v>4.0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="I11" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>29</v>
+      <c r="J11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12">
@@ -1170,7 +1314,7 @@
         <v>453000.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1">
         <v>453.0</v>
@@ -1182,19 +1326,22 @@
         <v>4.0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>29</v>
+      <c r="J12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13">
@@ -1202,31 +1349,34 @@
         <v>4100001.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1">
         <v>410.0</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="E13" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14">
@@ -1234,7 +1384,7 @@
         <v>4100002.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>410.0</v>
@@ -1243,19 +1393,22 @@
         <v>4.0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>29</v>
+      <c r="J14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15">
@@ -1263,7 +1416,7 @@
         <v>4100003.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1">
         <v>410.0</v>
@@ -1272,19 +1425,22 @@
         <v>4.0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I15" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>29</v>
+      <c r="J15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16">
@@ -1292,7 +1448,7 @@
         <v>330000.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1">
         <v>330.0</v>
@@ -1304,19 +1460,22 @@
         <v>4.0</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
@@ -1324,7 +1483,7 @@
         <v>422000.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1">
         <v>422.0</v>
@@ -1336,19 +1495,22 @@
         <v>4.0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G17" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J17" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K17" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -1356,7 +1518,7 @@
         <v>441000.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
         <v>441.0</v>
@@ -1368,19 +1530,22 @@
         <v>4.0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>29</v>
+      <c r="J18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19">
@@ -1388,7 +1553,7 @@
         <v>436000.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1">
         <v>436.0</v>
@@ -1400,19 +1565,22 @@
         <v>4.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>29</v>
+      <c r="J19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -1420,7 +1588,7 @@
         <v>432000.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1">
         <v>432.0</v>
@@ -1432,19 +1600,22 @@
         <v>4.0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G20" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="I20" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>29</v>
+      <c r="J20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21">
@@ -1452,7 +1623,7 @@
         <v>431000.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1">
         <v>431.0</v>
@@ -1464,19 +1635,22 @@
         <v>4.0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>29</v>
+      <c r="J21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22">
@@ -1484,31 +1658,34 @@
         <v>429000.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" s="1">
         <v>429.0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E22" s="1">
         <v>4.0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>29</v>
+      <c r="J22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23">
@@ -1516,31 +1693,34 @@
         <v>445000.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
         <v>445.0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1">
         <v>4.0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="I23" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>29</v>
+      <c r="J23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24">
@@ -1548,7 +1728,7 @@
         <v>415000.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1">
         <v>415.0</v>
@@ -1560,19 +1740,22 @@
         <v>4.0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G24" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J24" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K24" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25">
@@ -1580,7 +1763,7 @@
         <v>471000.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1">
         <v>471.0</v>
@@ -1592,19 +1775,22 @@
         <v>4.0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G25" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>29</v>
+      <c r="J25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26">
@@ -1612,7 +1798,7 @@
         <v>472000.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1">
         <v>472.0</v>
@@ -1624,19 +1810,22 @@
         <v>4.0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G26" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="I26" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>29</v>
+      <c r="J26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27">
@@ -1644,7 +1833,7 @@
         <v>425000.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1">
         <v>425.0</v>
@@ -1656,19 +1845,22 @@
         <v>4.0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G27" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>29</v>
+      <c r="J27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28">
@@ -1676,7 +1868,7 @@
         <v>413000.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28" s="1">
         <v>413.0</v>
@@ -1688,19 +1880,22 @@
         <v>4.0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J28" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="K28" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29">
@@ -1708,7 +1903,7 @@
         <v>420000.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C29" s="1">
         <v>420.0</v>
@@ -1720,19 +1915,22 @@
         <v>4.0</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J29" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="K29" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30">
@@ -1740,7 +1938,7 @@
         <v>427000.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C30" s="1">
         <v>427.0</v>
@@ -1750,7 +1948,7 @@
         <v>4.0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G30" s="1" t="b">
         <v>0</v>
@@ -1759,8 +1957,14 @@
       <c r="I30" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J30" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K30" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="31">
@@ -1768,7 +1972,7 @@
         <v>473000.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C31" s="1">
         <v>473.0</v>
@@ -1780,19 +1984,22 @@
         <v>4.0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J31" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="K31" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32">
@@ -1800,7 +2007,7 @@
         <v>423000.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C32" s="1">
         <v>423.0</v>
@@ -1812,19 +2019,22 @@
         <v>4.0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G32" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="I32" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>29</v>
+      <c r="J32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="33">
@@ -1832,31 +2042,34 @@
         <v>461000.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C33" s="1">
         <v>461.0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E33" s="1">
         <v>4.0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G33" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="I33" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>29</v>
+      <c r="J33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34">
@@ -1864,7 +2077,7 @@
         <v>433000.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34" s="1">
         <v>433.0</v>
@@ -1876,19 +2089,22 @@
         <v>4.0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G34" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>29</v>
+      <c r="J34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35">
@@ -1896,31 +2112,34 @@
         <v>434000.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C35" s="1">
         <v>434.0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="E35" s="1">
         <v>4.0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G35" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I35" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>29</v>
+      <c r="J35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36">
@@ -1928,7 +2147,7 @@
         <v>112001.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C36" s="1">
         <v>112.0</v>
@@ -1938,19 +2157,22 @@
         <v>4.0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J36" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K36" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37">
@@ -1958,7 +2180,7 @@
         <v>231001.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C37" s="1">
         <v>231.0</v>
@@ -1970,19 +2192,22 @@
         <v>4.0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="I37" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J37" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K37" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38">
@@ -1990,7 +2215,7 @@
         <v>232001.0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C38" s="1">
         <v>232.0</v>
@@ -2002,19 +2227,22 @@
         <v>4.0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="I38" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J38" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K38" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39">
@@ -2022,7 +2250,7 @@
         <v>251001.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1">
         <v>251.0</v>
@@ -2034,19 +2262,25 @@
         <v>4.0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G39" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="I39" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J39" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K39" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="40">
@@ -2054,7 +2288,7 @@
         <v>252001.0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1">
         <v>252.0</v>
@@ -2066,19 +2300,22 @@
         <v>4.0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G40" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="I40" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J40" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K40" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41">
@@ -2086,7 +2323,7 @@
         <v>343001.0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C41" s="1">
         <v>343.0</v>
@@ -2098,19 +2335,22 @@
         <v>4.0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G41" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="I41" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J41" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K41" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
@@ -2118,7 +2358,7 @@
         <v>341001.0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1">
         <v>341.0</v>
@@ -2130,19 +2370,22 @@
         <v>4.0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G42" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J42" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="K42" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
@@ -2150,7 +2393,7 @@
         <v>342001.0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C43" s="1">
         <v>342.0</v>
@@ -2162,19 +2405,22 @@
         <v>4.0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G43" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J43" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="K43" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44">
@@ -2182,7 +2428,7 @@
         <v>246001.0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C44" s="1">
         <v>246.0</v>
@@ -2194,19 +2440,22 @@
         <v>4.0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G44" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J44" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="K44" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45">
@@ -2214,7 +2463,7 @@
         <v>247001.0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C45" s="1">
         <v>247.0</v>
@@ -2226,19 +2475,22 @@
         <v>4.0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G45" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="I45" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J45" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="K45" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46">
@@ -2246,7 +2498,7 @@
         <v>261001.0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C46" s="1">
         <v>261.0</v>
@@ -2255,19 +2507,25 @@
         <v>4.0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G46" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="I46" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J46" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K46" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="47">
@@ -2275,7 +2533,7 @@
         <v>262001.0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C47" s="1">
         <v>262.0</v>
@@ -2284,19 +2542,22 @@
         <v>4.0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G47" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="I47" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J47" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K47" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48">
@@ -2304,7 +2565,7 @@
         <v>201002.0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C48" s="1">
         <v>201.0</v>
@@ -2313,13 +2574,16 @@
         <v>4.0</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="I48" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J48" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K48" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49">
@@ -2327,7 +2591,7 @@
         <v>202002.0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C49" s="1">
         <v>202.0</v>
@@ -2336,13 +2600,16 @@
         <v>4.0</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="I49" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J49" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K49" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50">
@@ -2350,7 +2617,7 @@
         <v>203002.0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C50" s="1">
         <v>203.0</v>
@@ -2359,13 +2626,16 @@
         <v>4.0</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="I50" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J50" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K50" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51">
@@ -2373,7 +2643,7 @@
         <v>251002.0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C51" s="1">
         <v>251.0</v>
@@ -2382,13 +2652,16 @@
         <v>4.0</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="I51" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J51" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="K51" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52">
@@ -2396,7 +2669,7 @@
         <v>252002.0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C52" s="1">
         <v>252.0</v>
@@ -2405,13 +2678,16 @@
         <v>4.0</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="I52" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J52" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="K52" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53">
@@ -2419,7 +2695,7 @@
         <v>253002.0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C53" s="1">
         <v>253.0</v>
@@ -2428,13 +2704,16 @@
         <v>4.0</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="I53" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J53" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="K53" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54">
@@ -2442,7 +2721,7 @@
         <v>221003.0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1">
         <v>221.0</v>
@@ -2451,13 +2730,16 @@
         <v>4.0</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="I54" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J54" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="K54" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55">
@@ -2465,7 +2747,7 @@
         <v>222003.0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C55" s="1">
         <v>222.0</v>
@@ -2474,13 +2756,16 @@
         <v>4.0</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="I55" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J55" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="K55" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56">
@@ -2488,7 +2773,7 @@
         <v>223003.0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C56" s="1">
         <v>223.0</v>
@@ -2497,13 +2782,16 @@
         <v>4.0</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="I56" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J56" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="K56" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57">
@@ -2511,7 +2799,7 @@
         <v>141004.0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C57" s="1">
         <v>141.0</v>
@@ -2520,13 +2808,16 @@
         <v>4.0</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="I57" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J57" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="K57" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58">
@@ -2534,7 +2825,7 @@
         <v>321004.0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C58" s="1">
         <v>321.0</v>
@@ -2543,13 +2834,16 @@
         <v>4.0</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="I58" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J58" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="K58" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59">
@@ -2557,7 +2851,7 @@
         <v>322004.0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C59" s="1">
         <v>322.0</v>
@@ -2566,13 +2860,16 @@
         <v>4.0</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="I59" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J59" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="K59" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60">
@@ -2580,7 +2877,7 @@
         <v>323004.0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C60" s="1">
         <v>323.0</v>
@@ -2589,13 +2886,16 @@
         <v>4.0</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="I60" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J60" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="K60" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61">
@@ -2603,7 +2903,7 @@
         <v>201005.0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="C61" s="1">
         <v>201.0</v>
@@ -2612,13 +2912,16 @@
         <v>4.0</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="I61" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J61" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="K61" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62">
@@ -2626,7 +2929,7 @@
         <v>202005.0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="C62" s="1">
         <v>202.0</v>
@@ -2635,13 +2938,16 @@
         <v>4.0</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="I62" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J62" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="K62" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63">
@@ -2649,7 +2955,7 @@
         <v>203005.0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="C63" s="1">
         <v>203.0</v>
@@ -2658,13 +2964,16 @@
         <v>4.0</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="I63" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J63" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="K63" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64">
@@ -2672,7 +2981,7 @@
         <v>201006.0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C64" s="1">
         <v>201.0</v>
@@ -2681,13 +2990,16 @@
         <v>4.0</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="I64" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J64" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="K64" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65">
@@ -2695,7 +3007,7 @@
         <v>348006.0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C65" s="1">
         <v>348.0</v>
@@ -2704,13 +3016,16 @@
         <v>4.0</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="I65" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J65" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="K65" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66">
@@ -2718,7 +3033,7 @@
         <v>301006.0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C66" s="1">
         <v>301.0</v>
@@ -2727,13 +3042,16 @@
         <v>4.0</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="I66" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J66" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="K66" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67">
@@ -2741,7 +3059,7 @@
         <v>304006.0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C67" s="1">
         <v>304.0</v>
@@ -2750,13 +3068,16 @@
         <v>4.0</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="I67" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J67" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="K67" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68">
@@ -2764,7 +3085,7 @@
         <v>305006.0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C68" s="1">
         <v>305.0</v>
@@ -2773,13 +3094,16 @@
         <v>4.0</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="I68" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J68" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="K68" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69">
@@ -2787,7 +3111,7 @@
         <v>111003.0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C69" s="1">
         <v>111.0</v>
@@ -2796,13 +3120,16 @@
         <v>4.0</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="I69" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J69" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="K69" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70">
@@ -2810,7 +3137,7 @@
         <v>113003.0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C70" s="1">
         <v>113.0</v>
@@ -2819,16 +3146,22 @@
         <v>4.0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="I70" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J70" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K70" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="71">
@@ -2836,7 +3169,7 @@
         <v>211007.0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C71" s="1">
         <v>211.0</v>
@@ -2845,13 +3178,16 @@
         <v>4.0</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="I71" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J71" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="K71" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72">
@@ -2859,7 +3195,7 @@
         <v>212007.0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C72" s="1">
         <v>212.0</v>
@@ -2868,13 +3204,16 @@
         <v>4.0</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="I72" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J72" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="K72" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73">
@@ -2882,7 +3221,7 @@
         <v>213007.0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="C73" s="1">
         <v>213.0</v>
@@ -2891,13 +3230,16 @@
         <v>4.0</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="I73" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J73" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="K73" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74">
@@ -2905,7 +3247,7 @@
         <v>121008.0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="C74" s="1">
         <v>121.0</v>
@@ -2920,13 +3262,16 @@
         <v>1</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="I74" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J74" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K74" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75">
@@ -2934,7 +3279,7 @@
         <v>122008.0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="C75" s="1">
         <v>122.0</v>
@@ -2949,13 +3294,16 @@
         <v>1</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="I75" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="J75" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K75" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76">
@@ -2963,7 +3311,7 @@
         <v>320008.0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="C76" s="1">
         <v>320.0</v>
@@ -2978,13 +3326,16 @@
         <v>1</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="I76" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J76" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K76" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77">
@@ -2992,7 +3343,7 @@
         <v>321008.0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="C77" s="1">
         <v>321.0</v>
@@ -3007,13 +3358,16 @@
         <v>1</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="I77" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J77" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="K77" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78">
@@ -3021,7 +3375,7 @@
         <v>253001.0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C78" s="1">
         <v>253.0</v>
@@ -3036,13 +3390,16 @@
         <v>1</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="I78" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J78" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="K78" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79">
@@ -3050,7 +3407,7 @@
         <v>281001.0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C79" s="1">
         <v>281.0</v>
@@ -3062,13 +3419,16 @@
         <v>4.0</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="I79" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J79" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="K79" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80">
@@ -3076,7 +3436,7 @@
         <v>256001.0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C80" s="1">
         <v>256.0</v>
@@ -3088,13 +3448,16 @@
         <v>4.0</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="I80" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J80" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="K80" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81">
@@ -3102,7 +3465,7 @@
         <v>282001.0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C81" s="1">
         <v>282.0</v>
@@ -3114,13 +3477,16 @@
         <v>4.0</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="I81" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J81" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="K81" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82">
@@ -3128,7 +3494,7 @@
         <v>307001.0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C82" s="1">
         <v>307.0</v>
@@ -3140,13 +3506,16 @@
         <v>4.0</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="I82" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J82" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="K82" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83">
@@ -3154,7 +3523,7 @@
         <v>316001.0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C83" s="1">
         <v>316.0</v>
@@ -3163,13 +3532,16 @@
         <v>4.0</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="I83" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J83" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K83" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84">
@@ -3177,7 +3549,7 @@
         <v>317001.0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C84" s="1">
         <v>317.0</v>
@@ -3189,13 +3561,16 @@
         <v>4.0</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="I84" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J84" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K84" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85">
@@ -3203,7 +3578,7 @@
         <v>320001.0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C85" s="1">
         <v>320.0</v>
@@ -3212,13 +3587,16 @@
         <v>4.0</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="I85" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J85" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="K85" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86">
@@ -3226,7 +3604,7 @@
         <v>345001.0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C86" s="1">
         <v>345.0</v>
@@ -3235,13 +3613,16 @@
         <v>4.0</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="I86" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J86" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K86" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87">
@@ -3249,7 +3630,7 @@
         <v>347001.0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C87" s="1">
         <v>347.0</v>
@@ -3258,13 +3639,16 @@
         <v>4.0</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="I87" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J87" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K87" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88">
@@ -3272,7 +3656,7 @@
         <v>348001.0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C88" s="1">
         <v>348.0</v>
@@ -3284,13 +3668,16 @@
         <v>4.0</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="I88" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J88" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K88" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89">
@@ -3298,7 +3685,7 @@
         <v>351001.0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C89" s="1">
         <v>351.0</v>
@@ -3307,13 +3694,16 @@
         <v>4.0</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="I89" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J89" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K89" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90">
@@ -3321,7 +3711,7 @@
         <v>352001.0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C90" s="1">
         <v>352.0</v>
@@ -3333,13 +3723,16 @@
         <v>4.0</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="I90" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J90" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K90" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91">
@@ -3347,7 +3740,7 @@
         <v>391001.0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C91" s="1">
         <v>391.0</v>
@@ -3356,13 +3749,16 @@
         <v>4.0</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="I91" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J91" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K91" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92">
@@ -3370,7 +3766,7 @@
         <v>392001.0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C92" s="1">
         <v>392.0</v>
@@ -3382,13 +3778,16 @@
         <v>4.0</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="I92" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J92" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K92" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93">
@@ -3396,7 +3795,7 @@
         <v>394001.0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C93" s="1">
         <v>394.0</v>
@@ -3405,13 +3804,16 @@
         <v>4.0</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="I93" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J93" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K93" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94">
@@ -3419,7 +3821,7 @@
         <v>395001.0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C94" s="1">
         <v>395.0</v>
@@ -3431,13 +3833,16 @@
         <v>4.0</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="I94" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J94" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K94" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95">
@@ -3445,7 +3850,7 @@
         <v>397001.0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C95" s="1">
         <v>397.0</v>
@@ -3454,13 +3859,16 @@
         <v>4.0</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="I95" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J95" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K95" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="96">
@@ -3468,7 +3876,7 @@
         <v>411001.0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C96" s="1">
         <v>411.0</v>
@@ -3477,13 +3885,16 @@
         <v>4.0</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="I96" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J96" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K96" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="97">
@@ -3491,7 +3902,7 @@
         <v>412001.0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C97" s="1">
         <v>412.0</v>
@@ -3500,13 +3911,16 @@
         <v>4.0</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="I97" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J97" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K97" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="98">
@@ -3514,7 +3928,7 @@
         <v>413001.0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C98" s="1">
         <v>413.0</v>
@@ -3523,13 +3937,16 @@
         <v>4.0</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="I98" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J98" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K98" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99">
@@ -3537,7 +3954,7 @@
         <v>414001.0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C99" s="1">
         <v>414.0</v>
@@ -3546,13 +3963,16 @@
         <v>4.0</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="I99" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J99" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K99" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100">
@@ -3560,7 +3980,7 @@
         <v>415001.0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C100" s="1">
         <v>415.0</v>
@@ -3569,13 +3989,16 @@
         <v>4.0</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="I100" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J100" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K100" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="101">
@@ -3583,7 +4006,7 @@
         <v>421001.0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C101" s="1">
         <v>421.0</v>
@@ -3592,13 +4015,16 @@
         <v>4.0</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="I101" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J101" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="K101" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102">
@@ -3606,7 +4032,7 @@
         <v>422001.0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C102" s="1">
         <v>422.0</v>
@@ -3615,13 +4041,16 @@
         <v>4.0</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="I102" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J102" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="K102" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103">
@@ -3629,7 +4058,7 @@
         <v>431001.0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C103" s="1">
         <v>431.0</v>
@@ -3638,13 +4067,16 @@
         <v>4.0</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
       <c r="I103" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J103" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K103" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104">
@@ -3652,7 +4084,7 @@
         <v>432001.0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C104" s="1">
         <v>432.0</v>
@@ -3661,13 +4093,16 @@
         <v>4.0</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="I104" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J104" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="K104" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105">
@@ -3675,7 +4110,7 @@
         <v>433001.0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C105" s="1">
         <v>433.0</v>
@@ -3684,13 +4119,16 @@
         <v>4.0</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="I105" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J105" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K105" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="106">
@@ -3698,7 +4136,7 @@
         <v>434001.0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C106" s="1">
         <v>434.0</v>
@@ -3707,13 +4145,16 @@
         <v>4.0</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="I106" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J106" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K106" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107">
@@ -3721,7 +4162,7 @@
         <v>441001.0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C107" s="1">
         <v>441.0</v>
@@ -3730,13 +4171,16 @@
         <v>4.0</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="I107" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J107" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="K107" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="108">
@@ -3744,7 +4188,7 @@
         <v>444001.0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C108" s="1">
         <v>444.0</v>
@@ -3753,13 +4197,16 @@
         <v>4.0</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="I108" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J108" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K108" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="109">
@@ -3767,7 +4214,7 @@
         <v>445001.0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C109" s="1">
         <v>445.0</v>
@@ -3776,13 +4223,16 @@
         <v>4.0</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="I109" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J109" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K109" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="110">
@@ -3790,7 +4240,7 @@
         <v>446001.0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C110" s="1">
         <v>446.0</v>
@@ -3799,13 +4249,16 @@
         <v>4.0</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="I110" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J110" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K110" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="111">
@@ -3813,7 +4266,7 @@
         <v>461001.0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C111" s="1">
         <v>461.0</v>
@@ -3822,13 +4275,16 @@
         <v>4.0</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="I111" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J111" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K111" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112">
@@ -3836,7 +4292,7 @@
         <v>462001.0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C112" s="1">
         <v>462.0</v>
@@ -3845,13 +4301,16 @@
         <v>4.0</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="I112" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J112" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="K112" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="113">
@@ -3859,7 +4318,7 @@
         <v>463001.0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C113" s="1">
         <v>463.0</v>
@@ -3868,13 +4327,16 @@
         <v>4.0</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="I113" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="J113" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K113" s="1" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114">
@@ -3882,7 +4344,7 @@
         <v>467001.0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C114" s="1">
         <v>467.0</v>
@@ -3891,13 +4353,16 @@
         <v>4.0</v>
       </c>
       <c r="H114" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I114" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K114" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="I114" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K114" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>